<commit_message>
All documents submission from supplier portal.
</commit_message>
<xml_diff>
--- a/SCTestData/SupplierCred.xlsx
+++ b/SCTestData/SupplierCred.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="38">
   <si>
     <t>UserName</t>
   </si>
@@ -81,6 +81,69 @@
   </si>
   <si>
     <t>Req_Supplier_On_17/12/18-19:04</t>
+  </si>
+  <si>
+    <t>Supplier_On_03/01/19-11:43</t>
+  </si>
+  <si>
+    <t>WorkGroup_On_03/01/19-11:43</t>
+  </si>
+  <si>
+    <t>Req_Supplier_On_03/01/19-11:44</t>
+  </si>
+  <si>
+    <t>Supplier_On_03/01/19-12:04</t>
+  </si>
+  <si>
+    <t>WorkGroup_On_03/01/19-12:04</t>
+  </si>
+  <si>
+    <t>Req_Supplier_On_03/01/19-12:05</t>
+  </si>
+  <si>
+    <t>Req_Supplier_On_04/01/19-17:48</t>
+  </si>
+  <si>
+    <t>Req_Supplier_On_04/01/19-17:49</t>
+  </si>
+  <si>
+    <t>Req_Supplier_On_04/01/19-17:59</t>
+  </si>
+  <si>
+    <t>Req_Supplier_On_04/01/19-18:07</t>
+  </si>
+  <si>
+    <t>Req_Supplier_On_04/01/19-18:14</t>
+  </si>
+  <si>
+    <t>Req_Supplier_On_04/01/19-18:17</t>
+  </si>
+  <si>
+    <t>Req_Supplier_On_04/01/19-18:25</t>
+  </si>
+  <si>
+    <t>Req_Supplier_On_04/01/19-18:32</t>
+  </si>
+  <si>
+    <t>Req_Supplier_On_04/01/19-18:35</t>
+  </si>
+  <si>
+    <t>Req_Supplier_On_04/01/19-18:39</t>
+  </si>
+  <si>
+    <t>Supplier_On_04/01/19-18:47</t>
+  </si>
+  <si>
+    <t>WorkGroup_On_04/01/19-18:47</t>
+  </si>
+  <si>
+    <t>Supplier_On_04/01/19-18:48</t>
+  </si>
+  <si>
+    <t>WorkGroup_On_04/01/19-18:48</t>
+  </si>
+  <si>
+    <t>Req_Supplier_On_04/01/19-18:48</t>
   </si>
 </sst>
 </file>
@@ -477,7 +540,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -486,10 +549,10 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create Requirements - Item . Link to supplier flow.
</commit_message>
<xml_diff>
--- a/SCTestData/SupplierCred.xlsx
+++ b/SCTestData/SupplierCred.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Data\SafetyChain-Test-Automation-Katalon\SCTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB56F92-1220-4B35-BF9A-3F29715E8376}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9298F6A2-3971-48B9-A7B2-5757318EAFA5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" xr2:uid="{C3001B69-76F0-4EAC-9C1F-7F69E5706FB2}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>UserName</t>
   </si>
@@ -50,119 +50,68 @@
     <t>WorkGroupName</t>
   </si>
   <si>
-    <t>Supplier_On_17/12/18-18:14</t>
-  </si>
-  <si>
-    <t>WorkGroup_On_17/12/18-18:14</t>
-  </si>
-  <si>
-    <t>Req_Supplier_On_17/12/18-18:15</t>
-  </si>
-  <si>
-    <t>password@</t>
-  </si>
-  <si>
-    <t>Supplier_On_17/12/18-18:39</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
-    <t>WorkGroup_On_17/12/18-18:39</t>
-  </si>
-  <si>
-    <t>Req_Supplier_On_17/12/18-18:40</t>
-  </si>
-  <si>
-    <t>Supplier_On_17/12/18-19:03</t>
-  </si>
-  <si>
-    <t>WorkGroup_On_17/12/18-19:03</t>
-  </si>
-  <si>
-    <t>Req_Supplier_On_17/12/18-19:04</t>
-  </si>
-  <si>
-    <t>Supplier_On_03/01/19-11:43</t>
-  </si>
-  <si>
-    <t>WorkGroup_On_03/01/19-11:43</t>
-  </si>
-  <si>
-    <t>Req_Supplier_On_03/01/19-11:44</t>
-  </si>
-  <si>
-    <t>Supplier_On_03/01/19-12:04</t>
-  </si>
-  <si>
-    <t>WorkGroup_On_03/01/19-12:04</t>
-  </si>
-  <si>
-    <t>Req_Supplier_On_03/01/19-12:05</t>
-  </si>
-  <si>
-    <t>Req_Supplier_On_04/01/19-17:48</t>
-  </si>
-  <si>
-    <t>Req_Supplier_On_04/01/19-17:49</t>
-  </si>
-  <si>
-    <t>Req_Supplier_On_04/01/19-17:59</t>
-  </si>
-  <si>
-    <t>Req_Supplier_On_04/01/19-18:07</t>
-  </si>
-  <si>
-    <t>Req_Supplier_On_04/01/19-18:14</t>
-  </si>
-  <si>
-    <t>Req_Supplier_On_04/01/19-18:17</t>
-  </si>
-  <si>
-    <t>Req_Supplier_On_04/01/19-18:25</t>
-  </si>
-  <si>
-    <t>Req_Supplier_On_04/01/19-18:32</t>
-  </si>
-  <si>
-    <t>Req_Supplier_On_04/01/19-18:35</t>
-  </si>
-  <si>
-    <t>Req_Supplier_On_04/01/19-18:39</t>
-  </si>
-  <si>
-    <t>Supplier_On_04/01/19-18:47</t>
-  </si>
-  <si>
-    <t>WorkGroup_On_04/01/19-18:47</t>
-  </si>
-  <si>
-    <t>Supplier_On_04/01/19-18:48</t>
-  </si>
-  <si>
-    <t>WorkGroup_On_04/01/19-18:48</t>
-  </si>
-  <si>
-    <t>Req_Supplier_On_04/01/19-18:48</t>
+    <t>FormTask</t>
+  </si>
+  <si>
+    <t>DocTask</t>
+  </si>
+  <si>
+    <t>ACKTask</t>
+  </si>
+  <si>
+    <t>ItemName</t>
+  </si>
+  <si>
+    <t>FormTask1</t>
+  </si>
+  <si>
+    <t>DocTask1</t>
+  </si>
+  <si>
+    <t>ACKTask1</t>
+  </si>
+  <si>
+    <t>AUTO_TEST_RESTORE_DOCUMENT_ON_03/01/2019-12:40:27</t>
+  </si>
+  <si>
+    <t>Supplier_On_11/01/19-14:15</t>
+  </si>
+  <si>
+    <t>WorkGroup_11/01/19-14:15</t>
+  </si>
+  <si>
+    <t>Req_Supplier_On_11/01/19-14:16</t>
+  </si>
+  <si>
+    <t>TestFormTask_11/01/19-14:17</t>
+  </si>
+  <si>
+    <t>Req_Supplier_On_11/01/19-14:18</t>
+  </si>
+  <si>
+    <t>TestACKTask_11/01/19-14:19</t>
+  </si>
+  <si>
+    <t>TestFormTask_11/01/19-14:20</t>
+  </si>
+  <si>
+    <t>TestDocTask_11/01/19-14:21</t>
+  </si>
+  <si>
+    <t>jj</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -185,16 +134,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -507,21 +453,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA95E537-9AEB-4521-916E-7A54A0A646F7}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="1" max="1" width="21.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="28.28515625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="25.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -537,22 +485,64 @@
       <c r="E1" t="s">
         <v>5</v>
       </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update - Task Schedular.
</commit_message>
<xml_diff>
--- a/SCTestData/SupplierCred.xlsx
+++ b/SCTestData/SupplierCred.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="179">
   <si>
     <t>UserName</t>
   </si>
@@ -225,6 +225,348 @@
   </si>
   <si>
     <t>WorkGroup_06/02/19-18:18</t>
+  </si>
+  <si>
+    <t>WorkGroup_19/02/19-12:31</t>
+  </si>
+  <si>
+    <t>Supplier_19/02/19-13:00</t>
+  </si>
+  <si>
+    <t>WorkGroup_19/02/19-13:00</t>
+  </si>
+  <si>
+    <t>Supplier_19/02/19-13:01</t>
+  </si>
+  <si>
+    <t>WorkGroup_19/02/19-13:01</t>
+  </si>
+  <si>
+    <t>SuppReq_19/02/19-13:02</t>
+  </si>
+  <si>
+    <t>TestACKTask_19/02/19-13:02</t>
+  </si>
+  <si>
+    <t>TestFormTask_19/02/19-13:03</t>
+  </si>
+  <si>
+    <t>TestDocTask_19/02/19-13:03</t>
+  </si>
+  <si>
+    <t>ItemReq_19/02/19-13:04</t>
+  </si>
+  <si>
+    <t>TestACKTask_19/02/19-13:05</t>
+  </si>
+  <si>
+    <t>TestFormTask_19/02/19-13:06</t>
+  </si>
+  <si>
+    <t>TestDocTask_19/02/19-13:07</t>
+  </si>
+  <si>
+    <t>Supplier_19/02/19-13:52</t>
+  </si>
+  <si>
+    <t>WorkGroup_19/02/19-13:52</t>
+  </si>
+  <si>
+    <t>SuppReq_19/02/19-13:53</t>
+  </si>
+  <si>
+    <t>TestACKTask_19/02/19-13:54</t>
+  </si>
+  <si>
+    <t>TestFormTask_19/02/19-13:54</t>
+  </si>
+  <si>
+    <t>TestDocTask_19/02/19-13:55</t>
+  </si>
+  <si>
+    <t>ItemReq_19/02/19-13:56</t>
+  </si>
+  <si>
+    <t>TestACKTask_19/02/19-13:56</t>
+  </si>
+  <si>
+    <t>TestFormTask_19/02/19-13:57</t>
+  </si>
+  <si>
+    <t>TestDocTask_19/02/19-13:58</t>
+  </si>
+  <si>
+    <t>WorkGroup_20/02/19-14:44</t>
+  </si>
+  <si>
+    <t>WorkGroup_20/02/19-15:49</t>
+  </si>
+  <si>
+    <t>Supplier_20/02/19-16:00</t>
+  </si>
+  <si>
+    <t>WorkGroup_20/02/19-16:00</t>
+  </si>
+  <si>
+    <t>Supplier_20/02/19-16:01</t>
+  </si>
+  <si>
+    <t>WorkGroup_20/02/19-16:01</t>
+  </si>
+  <si>
+    <t>SuppReq_20/02/19-16:01</t>
+  </si>
+  <si>
+    <t>TestACKTask_20/02/19-16:02</t>
+  </si>
+  <si>
+    <t>TestFormTask_20/02/19-16:03</t>
+  </si>
+  <si>
+    <t>TestDocTask_20/02/19-16:03</t>
+  </si>
+  <si>
+    <t>ItemReq_20/02/19-16:04</t>
+  </si>
+  <si>
+    <t>Supplier_20/02/19-16:42</t>
+  </si>
+  <si>
+    <t>WorkGroup_20/02/19-16:42</t>
+  </si>
+  <si>
+    <t>SuppReq_20/02/19-16:43</t>
+  </si>
+  <si>
+    <t>TestACKTask_20/02/19-16:43</t>
+  </si>
+  <si>
+    <t>TestFormTask_20/02/19-16:44</t>
+  </si>
+  <si>
+    <t>TestDocTask_20/02/19-16:45</t>
+  </si>
+  <si>
+    <t>ItemReq_20/02/19-16:46</t>
+  </si>
+  <si>
+    <t>TestACKTask_20/02/19-16:46</t>
+  </si>
+  <si>
+    <t>TestFormTask_20/02/19-16:47</t>
+  </si>
+  <si>
+    <t>TestDocTask_20/02/19-16:48</t>
+  </si>
+  <si>
+    <t>WorkGroup_21/02/19-14:19</t>
+  </si>
+  <si>
+    <t>WorkGroup_21/02/19-14:28</t>
+  </si>
+  <si>
+    <t>WorkGroup_21/02/19-15:13</t>
+  </si>
+  <si>
+    <t>WorkGroup_25/02/19-17:14</t>
+  </si>
+  <si>
+    <t>Supplier_26/02/19-11:59</t>
+  </si>
+  <si>
+    <t>WorkGroup_26/02/19-11:59</t>
+  </si>
+  <si>
+    <t>Supplier_26/02/19-12:00</t>
+  </si>
+  <si>
+    <t>WorkGroup_26/02/19-12:00</t>
+  </si>
+  <si>
+    <t>SuppReq_26/02/19-12:00</t>
+  </si>
+  <si>
+    <t>TestACKTask_26/02/19-12:01</t>
+  </si>
+  <si>
+    <t>TestFormTask_26/02/19-12:01</t>
+  </si>
+  <si>
+    <t>TestDocTask_26/02/19-12:02</t>
+  </si>
+  <si>
+    <t>ItemReq_26/02/19-12:03</t>
+  </si>
+  <si>
+    <t>TestACKTask_26/02/19-12:04</t>
+  </si>
+  <si>
+    <t>TestFormTask_26/02/19-12:04</t>
+  </si>
+  <si>
+    <t>TestDocTask_26/02/19-12:05</t>
+  </si>
+  <si>
+    <t>Supplier_28/02/19-16:10</t>
+  </si>
+  <si>
+    <t>WorkGroup_28/02/19-16:10</t>
+  </si>
+  <si>
+    <t>Supplier_28/02/19-16:11</t>
+  </si>
+  <si>
+    <t>WorkGroup_28/02/19-16:11</t>
+  </si>
+  <si>
+    <t>SuppReq_28/02/19-16:11</t>
+  </si>
+  <si>
+    <t>TestACKTask_28/02/19-16:12</t>
+  </si>
+  <si>
+    <t>TestFormTask_28/02/19-16:12</t>
+  </si>
+  <si>
+    <t>TestDocTask_28/02/19-16:13</t>
+  </si>
+  <si>
+    <t>ItemReq_28/02/19-16:14</t>
+  </si>
+  <si>
+    <t>TestACKTask_28/02/19-16:15</t>
+  </si>
+  <si>
+    <t>TestFormTask_28/02/19-16:15</t>
+  </si>
+  <si>
+    <t>TestDocTask_28/02/19-16:16</t>
+  </si>
+  <si>
+    <t>WorkGroup_28/02/19-17:19</t>
+  </si>
+  <si>
+    <t>WorkGroup_28/02/19-17:49</t>
+  </si>
+  <si>
+    <t>WorkGroup_28/02/19-18:18</t>
+  </si>
+  <si>
+    <t>WorkGroup_01/03/19-11:34</t>
+  </si>
+  <si>
+    <t>WorkGroup_01/03/19-13:07</t>
+  </si>
+  <si>
+    <t>WorkGroup_01/03/19-15:05</t>
+  </si>
+  <si>
+    <t>WorkGroup_01/03/19-15:26</t>
+  </si>
+  <si>
+    <t>WorkGroup_01/03/19-15:57</t>
+  </si>
+  <si>
+    <t>Supplier_05/03/19-11:58</t>
+  </si>
+  <si>
+    <t>WorkGroup_05/03/19-11:58</t>
+  </si>
+  <si>
+    <t>SuppReq_05/03/19-11:59</t>
+  </si>
+  <si>
+    <t>TestACKTask_05/03/19-12:00</t>
+  </si>
+  <si>
+    <t>TestFormTask_05/03/19-12:00</t>
+  </si>
+  <si>
+    <t>TestDocTask_05/03/19-12:01</t>
+  </si>
+  <si>
+    <t>ItemReq_05/03/19-12:02</t>
+  </si>
+  <si>
+    <t>TestACKTask_05/03/19-12:02</t>
+  </si>
+  <si>
+    <t>TestFormTask_05/03/19-12:03</t>
+  </si>
+  <si>
+    <t>TestDocTask_05/03/19-12:04</t>
+  </si>
+  <si>
+    <t>Supplier_05/03/19-14:31</t>
+  </si>
+  <si>
+    <t>WorkGroup_05/03/19-14:31</t>
+  </si>
+  <si>
+    <t>SuppReq_05/03/19-14:32</t>
+  </si>
+  <si>
+    <t>TestACKTask_05/03/19-14:33</t>
+  </si>
+  <si>
+    <t>TestFormTask_05/03/19-14:33</t>
+  </si>
+  <si>
+    <t>TestDocTask_05/03/19-14:34</t>
+  </si>
+  <si>
+    <t>ItemReq_05/03/19-14:35</t>
+  </si>
+  <si>
+    <t>TestACKTask_05/03/19-14:35</t>
+  </si>
+  <si>
+    <t>TestFormTask_05/03/19-14:36</t>
+  </si>
+  <si>
+    <t>TestDocTask_05/03/19-14:37</t>
+  </si>
+  <si>
+    <t>Supplier_05/03/19-15:02</t>
+  </si>
+  <si>
+    <t>WorkGroup_05/03/19-15:02</t>
+  </si>
+  <si>
+    <t>SuppReq_05/03/19-15:03</t>
+  </si>
+  <si>
+    <t>TestACKTask_05/03/19-15:04</t>
+  </si>
+  <si>
+    <t>TestFormTask_05/03/19-15:04</t>
+  </si>
+  <si>
+    <t>TestDocTask_05/03/19-15:05</t>
+  </si>
+  <si>
+    <t>ItemReq_05/03/19-15:06</t>
+  </si>
+  <si>
+    <t>TestACKTask_05/03/19-15:06</t>
+  </si>
+  <si>
+    <t>TestFormTask_05/03/19-15:07</t>
+  </si>
+  <si>
+    <t>TestDocTask_05/03/19-15:08</t>
+  </si>
+  <si>
+    <t>WorkGroup_08/03/19-12:23</t>
+  </si>
+  <si>
+    <t>WorkGroup_08/03/19-13:12</t>
+  </si>
+  <si>
+    <t>WorkGroup_08/03/19-14:21</t>
+  </si>
+  <si>
+    <t>WorkGroup_08/03/19-14:43</t>
   </si>
 </sst>
 </file>
@@ -633,7 +975,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>165</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -642,31 +984,31 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>167</v>
       </c>
       <c r="E2" t="s">
-        <v>64</v>
+        <v>178</v>
       </c>
       <c r="F2" t="s">
-        <v>58</v>
+        <v>169</v>
       </c>
       <c r="G2" t="s">
-        <v>59</v>
+        <v>170</v>
       </c>
       <c r="H2" t="s">
-        <v>57</v>
+        <v>168</v>
       </c>
       <c r="I2" t="s">
-        <v>60</v>
+        <v>171</v>
       </c>
       <c r="J2" t="s">
-        <v>62</v>
+        <v>173</v>
       </c>
       <c r="K2" t="s">
-        <v>63</v>
+        <v>174</v>
       </c>
       <c r="L2" t="s">
-        <v>61</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>